<commit_message>
using value from Read excel file in testcase
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Testdata.xlsx
+++ b/src/test/resources/testdata/Testdata.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="login" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Logintest" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -107,8 +107,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -247,38 +251,38 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.92"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>2175506455</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="2" t="n">
         <v>8426</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="2" t="n">
         <v>1175506455</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="2" t="n">
         <v>8426</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="2" t="n">
         <v>9175506455</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="2" t="n">
         <v>8426</v>
       </c>
     </row>

</xml_diff>